<commit_message>
Added sequentional orthogonalization version to check_ort/run.py
</commit_message>
<xml_diff>
--- a/experiments/pg/start_from_m1_6_1_max_step_2_step_num_4_ret_norm_gamma_0_1/oracle_buffer.xlsx
+++ b/experiments/pg/start_from_m1_6_1_max_step_2_step_num_4_ret_norm_gamma_0_1/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C291"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>[-1, 5, 0]</t>
+          <t>[1, 2, -1]</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.5101362612319004</v>
+        <v>4.986757427146849</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>[-2, 5, 0]</t>
+          <t>[1, 2, 1]</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.5080793864935131</v>
+        <v>4.999250248460044</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>[-5, 5, -1]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.4447621801987933</v>
+        <v>8.608650936808958</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>[-1, 0, 1]</t>
+          <t>[-1, 4, -3]</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>15.58595287876404</v>
+        <v>1.304632807452957</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>[2, 3, 1]</t>
+          <t>[-1, 2, -3]</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2.560982016640212</v>
+        <v>5.177871157936687</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>[-1, 2, 2]</t>
+          <t>[-2, 5, 1]</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5.250032650881911</v>
+        <v>0.5101579424287024</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[0, 2, 2]</t>
+          <t>[-6, 7, 1]</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>5.230420779607464</v>
+        <v>0.1213201456348434</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>[-4, 2, 1]</t>
+          <t>[-1, 0, 1]</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>4.436469666782642</v>
+        <v>15.58595289834594</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>[1, 2, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>4.994555182017475</v>
+        <v>12.91873297179849</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[0, 3, 1]</t>
+          <t>[-1, 3, 0]</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2.798329361389709</v>
+        <v>2.810309843771755</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[2, 4, 1]</t>
+          <t>[-4, 6, 3]</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1.227439417921204</v>
+        <v>0.1495708588717729</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[-1, 1, 2]</t>
+          <t>[-4, 5, 3]</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>9.331973275546934</v>
+        <v>0.4711538809917316</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[-4, 6, 3]</t>
+          <t>[0, 3, 1]</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0.1495708588686223</v>
+        <v>2.798329361593266</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[-5, 6, 3]</t>
+          <t>[0, 3, -1]</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0.143160192528317</v>
+        <v>2.780298530073265</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[-2, 2, 0]</t>
+          <t>[-6, 6, 1]</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>5.099905900647289</v>
+        <v>0.1394436749446289</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[0, 4, -1]</t>
+          <t>[-1, 3, -3]</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1.316142723025028</v>
+        <v>2.768508689785585</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[-3, 0, 1]</t>
+          <t>[-1, 0, 3]</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>11.26763255968622</v>
+        <v>15.18121019135254</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[1, 4, 3]</t>
+          <t>[-3, 4, -3]</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1.290633993913607</v>
+        <v>1.239996436977657</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[-6, 6, 1]</t>
+          <t>[-5, 3, 1]</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0.1394436749446289</v>
+        <v>2.301498566540119</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[-1, 4, -3]</t>
+          <t>[-5, 5, -1]</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>1.304632807322218</v>
+        <v>0.4447621802331836</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[-3, 4, -3]</t>
+          <t>[-1, 0, -1]</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>1.239996437525117</v>
+        <v>15.39679870666104</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>[-5, 3, 1]</t>
+          <t>[-5, 5, 1]</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>2.30149856655868</v>
+        <v>0.4507917971354258</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>[-3, 1, 1]</t>
+          <t>[-1, 3, -1]</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>8.025266057781092</v>
+        <v>2.798624292166643</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[-1, 2, -3]</t>
+          <t>[-2, 0, 1]</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>5.177871157614998</v>
+        <v>13.5870210573229</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>[0, 2, -1]</t>
+          <t>[-1, 7, -3]</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>5.190229770716156</v>
+        <v>0.1133735369123567</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>[-2, 5, 1]</t>
+          <t>[0, 2, 1]</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.5101579424161142</v>
+        <v>5.22559692771903</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[-3, 2, 0]</t>
+          <t>[-1, 5, 2]</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>4.807343614166546</v>
+        <v>0.5124333795674501</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[-3, 3, 2]</t>
+          <t>[0, 2, -1]</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>2.646484710681149</v>
+        <v>5.190229769392185</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[1, 2, 1]</t>
+          <t>[-3, 3, 2]</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4.999250249141519</v>
+        <v>2.646484710949548</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[3, 4, 1]</t>
+          <t>[2, 4, 1]</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1.156479455202905</v>
+        <v>1.227439417960584</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[0, 6, -5]</t>
+          <t>[-1, 7, -5]</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0.1151578486713284</v>
+        <v>0.09734249401032234</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[-1, 1, -1]</t>
+          <t>[-3, 0, 1]</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>9.300352064960187</v>
+        <v>11.26763255960378</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[1, 2, 2]</t>
+          <t>[-1, -2, 1]</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>5.017274403283408</v>
+        <v>6.791427325093312</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[-2, 4, 0]</t>
+          <t>[-3, 1, 1]</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>1.317798943033378</v>
+        <v>8.0252660584596</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[0, 3, -1]</t>
+          <t>[-5, 6, -1]</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2.780298530266545</v>
+        <v>0.1453463200243862</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[-2, 2, -1]</t>
+          <t>[-6, 6, -1]</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5.080849186679457</v>
+        <v>0.1370722988741251</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[-1, 3, -2]</t>
+          <t>[-1, 2, 2]</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2.784225019508755</v>
+        <v>5.250032650574821</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>[-4, 4, 3]</t>
+          <t>[-2, 4, 0]</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1.208960875751625</v>
+        <v>1.317798943033378</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>[-1, 3, 0]</t>
+          <t>[-2, 2, 0]</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>2.810309843696943</v>
+        <v>5.099905900652971</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>[-2, 3, 0]</t>
+          <t>[0, 6, -1]</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>2.757101677409204</v>
+        <v>0.1446398312297908</v>
       </c>
     </row>
     <row r="173">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0.1284162878126478</v>
+        <v>0.1284162878130437</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>[0, 7, -3]</t>
+          <t>[0, 4, -3]</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.1079794659386595</v>
+        <v>1.295942700469052</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>[-1, 0, 0]</t>
+          <t>[-2, 5, -1]</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>15.56833547950951</v>
+        <v>0.501679787075918</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[-1, 5, -3]</t>
+          <t>[-2, 3, -1]</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0.4846099487344858</v>
+        <v>2.745316190308827</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>[-1, 5, -2]</t>
+          <t>[-1, 3, -2]</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0.4945353651139758</v>
+        <v>2.784225019508755</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>[0, 3, 0]</t>
+          <t>[-4, 4, 3]</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>2.790245288110522</v>
+        <v>1.208960875751625</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>[0, 2, 1]</t>
+          <t>[-3, 3, 0]</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>5.225596927030887</v>
+        <v>2.64338159981973</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[0, 3, 3]</t>
+          <t>[-1, 1, 2]</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>2.795720124610749</v>
+        <v>9.331973277589849</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[-5, 6, 0]</t>
+          <t>[-3, 2, 2]</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.1479639904417516</v>
+        <v>4.813004675572612</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>[-7, 6, 0]</t>
+          <t>[0, 5, 3]</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0.129071938680603</v>
+        <v>0.5034976198890866</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[-2, 0, 1]</t>
+          <t>[-4, 2, 1]</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>13.58702106668736</v>
+        <v>4.436469666044751</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>[-1, 0, -1]</t>
+          <t>[-2, 2, -1]</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>15.39679870371111</v>
+        <v>5.080849187107782</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[-1, 3, -1]</t>
+          <t>[0, 0, 1]</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>2.798624292805943</v>
+        <v>15.3267182999025</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[-1, 5, 2]</t>
+          <t>[-3, 4, 5]</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0.5124333795766555</v>
+        <v>1.253316869387955</v>
       </c>
     </row>
     <row r="187">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[-2, 5, 2]</t>
+          <t>[-1, 1, 3]</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.5083599711464163</v>
+        <v>9.279892401839311</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[-1, 2, -2]</t>
+          <t>[0, 2, 2]</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>5.204809832728178</v>
+        <v>5.230420777589211</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>[-1, -1, 1]</t>
+          <t>[-1, 1, -1]</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>12.08448259354965</v>
+        <v>9.300352059366455</v>
       </c>
     </row>
     <row r="191">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>[-1, 2, 3]</t>
+          <t>[-2, 2, 3]</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>5.23357826854647</v>
+        <v>5.083003994158909</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>[-1, 0, 3]</t>
+          <t>[3, 4, 1]</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>15.18121019342151</v>
+        <v>1.15647945509265</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>[1, 4, -1]</t>
+          <t>[4, 4, 1]</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>1.28156450334296</v>
+        <v>1.076519832344164</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>[1, 5, -1]</t>
+          <t>[-3, 2, 0]</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0.4813602723602805</v>
+        <v>4.807343613425881</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>[-5, 5, 1]</t>
+          <t>[-1, 2, 3]</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.4507917971314129</v>
+        <v>5.233578269559516</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>[-1, -2, 1]</t>
+          <t>[2, 6, 1]</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>6.791427325144901</v>
+        <v>0.1342063216705103</v>
       </c>
     </row>
     <row r="200">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>[1, 0, 1]</t>
+          <t>[-1, 1, 0]</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>12.91873297274447</v>
+        <v>9.346353453816347</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>[1, 2, -1]</t>
+          <t>[-1, 0, 0]</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>4.986757428218821</v>
+        <v>15.56833548160802</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>[0, 0, 1]</t>
+          <t>[-1, 2, -2]</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>15.32671829450645</v>
+        <v>5.204809831831199</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>[-2, 2, 2]</t>
+          <t>[-3, 5, 2]</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>5.098096156181288</v>
+        <v>0.4956421854816734</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>[-1, 1, 0]</t>
+          <t>[-1, 2, 4]</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>9.346353454531581</v>
+        <v>5.212528518462868</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>[0, 3, 2]</t>
+          <t>[-1, -1, 1]</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>2.80053333796698</v>
+        <v>12.0844825886097</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>[-3, 5, 0]</t>
+          <t>[3, 2, 1]</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>0.4959245327043925</v>
+        <v>4.245172988668764</v>
       </c>
     </row>
     <row r="208">
@@ -3133,7 +3133,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2.698511154281723</v>
+        <v>2.698511154149754</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>[3, 2, 1]</t>
+          <t>[-2, 3, 2]</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>4.245172989635759</v>
+        <v>2.757831098416188</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 2, 3]</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>8.608650935683501</v>
+        <v>5.029870147696805</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>[-3, 2, 2]</t>
+          <t>[-2, 2, 2]</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>4.813004675774987</v>
+        <v>5.098096156278123</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>[0, 4, 3]</t>
+          <t>[-3, 2, 3]</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>1.325431194010192</v>
+        <v>4.801702717739232</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>[0, 2, 3]</t>
+          <t>[2, 2, 1]</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>5.22186551331448</v>
+        <v>4.648356624254395</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[-5, 4, 2]</t>
+          <t>[1, 2, 0]</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>1.136114593312411</v>
+        <v>4.994555183109602</v>
       </c>
     </row>
     <row r="215">
@@ -3220,999 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>[-1, 3, -3]</t>
+          <t>[1, 2, 2]</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>2.768508689555366</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>[0, 5, 3]</t>
-        </is>
-      </c>
-      <c r="C216" t="n">
-        <v>0.503497619805849</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>[2, 2, 1]</t>
-        </is>
-      </c>
-      <c r="C217" t="n">
-        <v>4.648356624530097</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>[-5, 4, 0]</t>
-        </is>
-      </c>
-      <c r="C218" t="n">
-        <v>1.135184438906618</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>[1, 4, -3]</t>
-        </is>
-      </c>
-      <c r="C219" t="n">
-        <v>1.265425016841788</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>[-1, 1, 3]</t>
-        </is>
-      </c>
-      <c r="C220" t="n">
-        <v>9.279892401260245</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>[-7, 4, 1]</t>
-        </is>
-      </c>
-      <c r="C221" t="n">
-        <v>0.9471586525506499</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>[-2, 2, 3]</t>
-        </is>
-      </c>
-      <c r="C222" t="n">
-        <v>5.083003994026988</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>[-2, 3, -1]</t>
-        </is>
-      </c>
-      <c r="C223" t="n">
-        <v>2.745316190614011</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>[-1, 2, 4]</t>
-        </is>
-      </c>
-      <c r="C224" t="n">
-        <v>5.212528518100963</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1" t="n">
-        <v>223</v>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>[-1, 3, 4]</t>
-        </is>
-      </c>
-      <c r="C225" t="n">
-        <v>2.793248752034283</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>[0, 2, 0]</t>
-        </is>
-      </c>
-      <c r="C226" t="n">
-        <v>5.209240326150891</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>[-2, 4, -2]</t>
-        </is>
-      </c>
-      <c r="C227" t="n">
-        <v>1.297949311011526</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" s="1" t="n">
-        <v>226</v>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>[-3, 2, 3]</t>
-        </is>
-      </c>
-      <c r="C228" t="n">
-        <v>4.801702717563242</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" s="1" t="n">
-        <v>227</v>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>[-1, 2, 5]</t>
-        </is>
-      </c>
-      <c r="C229" t="n">
-        <v>5.19044080474827</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1" t="n">
-        <v>228</v>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>[-2, 4, 2]</t>
-        </is>
-      </c>
-      <c r="C230" t="n">
-        <v>1.318490118335251</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>[-1, 4, 4]</t>
-        </is>
-      </c>
-      <c r="C231" t="n">
-        <v>1.323936564509012</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>[-1, 4, -4]</t>
-        </is>
-      </c>
-      <c r="C232" t="n">
-        <v>1.293788764141417</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" s="1" t="n">
-        <v>231</v>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>[-1, 4, 5]</t>
-        </is>
-      </c>
-      <c r="C233" t="n">
-        <v>1.315359030619805</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1" t="n">
-        <v>232</v>
-      </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>[0, 4, 2]</t>
-        </is>
-      </c>
-      <c r="C234" t="n">
-        <v>1.328964370487933</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1" t="n">
-        <v>233</v>
-      </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>[-3, 5, 2]</t>
-        </is>
-      </c>
-      <c r="C235" t="n">
-        <v>0.4956421854872817</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1" t="n">
-        <v>234</v>
-      </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>[-3, 5, 4]</t>
-        </is>
-      </c>
-      <c r="C236" t="n">
-        <v>0.4845210296724473</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="n">
-        <v>235</v>
-      </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>[-1, 6, -4]</t>
-        </is>
-      </c>
-      <c r="C237" t="n">
-        <v>0.1241720277814379</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1" t="n">
-        <v>236</v>
-      </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>[0, 4, 4]</t>
-        </is>
-      </c>
-      <c r="C238" t="n">
-        <v>1.318897102745103</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="B239" t="inlineStr">
-        <is>
-          <t>[-2, 4, 3]</t>
-        </is>
-      </c>
-      <c r="C239" t="n">
-        <v>1.312663444272024</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1" t="n">
-        <v>238</v>
-      </c>
-      <c r="B240" t="inlineStr">
-        <is>
-          <t>[0, 4, -2]</t>
-        </is>
-      </c>
-      <c r="C240" t="n">
-        <v>1.306565157308948</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1" t="n">
-        <v>239</v>
-      </c>
-      <c r="B241" t="inlineStr">
-        <is>
-          <t>[1, 2, 3]</t>
-        </is>
-      </c>
-      <c r="C241" t="n">
-        <v>5.029870147186172</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>[1, 4, 4]</t>
-        </is>
-      </c>
-      <c r="C242" t="n">
-        <v>1.287544510272905</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1" t="n">
-        <v>241</v>
-      </c>
-      <c r="B243" t="inlineStr">
-        <is>
-          <t>[-2, 3, 2]</t>
-        </is>
-      </c>
-      <c r="C243" t="n">
-        <v>2.757831098334988</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" s="1" t="n">
-        <v>242</v>
-      </c>
-      <c r="B244" t="inlineStr">
-        <is>
-          <t>[1, 3, 2]</t>
-        </is>
-      </c>
-      <c r="C244" t="n">
-        <v>2.71208005955836</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1" t="n">
-        <v>243</v>
-      </c>
-      <c r="B245" t="inlineStr">
-        <is>
-          <t>[0, 4, -3]</t>
-        </is>
-      </c>
-      <c r="C245" t="n">
-        <v>1.295942700065763</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1" t="n">
-        <v>244</v>
-      </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>[-2, 4, 4]</t>
-        </is>
-      </c>
-      <c r="C246" t="n">
-        <v>1.304538786524339</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1" t="n">
-        <v>245</v>
-      </c>
-      <c r="B247" t="inlineStr">
-        <is>
-          <t>[-3, 7, 4]</t>
-        </is>
-      </c>
-      <c r="C247" t="n">
-        <v>0.1290532110249593</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1" t="n">
-        <v>246</v>
-      </c>
-      <c r="B248" t="inlineStr">
-        <is>
-          <t>[1, 5, 3]</t>
-        </is>
-      </c>
-      <c r="C248" t="n">
-        <v>0.4885199807693701</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="n">
-        <v>247</v>
-      </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>[-1, 6, 5]</t>
-        </is>
-      </c>
-      <c r="C249" t="n">
-        <v>0.1436795024627673</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" s="1" t="n">
-        <v>248</v>
-      </c>
-      <c r="B250" t="inlineStr">
-        <is>
-          <t>[-3, 4, 5]</t>
-        </is>
-      </c>
-      <c r="C250" t="n">
-        <v>1.253316869375455</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" s="1" t="n">
-        <v>249</v>
-      </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>[-1, 3, 5]</t>
-        </is>
-      </c>
-      <c r="C251" t="n">
-        <v>2.781592621400557</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>[-2, 6, 2]</t>
-        </is>
-      </c>
-      <c r="C252" t="n">
-        <v>0.1605404380136037</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" s="1" t="n">
-        <v>251</v>
-      </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>[-2, 6, 3]</t>
-        </is>
-      </c>
-      <c r="C253" t="n">
-        <v>0.1562791318061174</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" s="1" t="n">
-        <v>252</v>
-      </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>[-1, 5, 5]</t>
-        </is>
-      </c>
-      <c r="C254" t="n">
-        <v>0.4946892525655325</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" s="1" t="n">
-        <v>253</v>
-      </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t>[0, 7, 3]</t>
-        </is>
-      </c>
-      <c r="C255" t="n">
-        <v>0.1343220619765621</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" s="1" t="n">
-        <v>254</v>
-      </c>
-      <c r="B256" t="inlineStr">
-        <is>
-          <t>[-1, 7, 5]</t>
-        </is>
-      </c>
-      <c r="C256" t="n">
-        <v>0.1252497449201891</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" s="1" t="n">
-        <v>255</v>
-      </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>[0, 7, 2]</t>
-        </is>
-      </c>
-      <c r="C257" t="n">
-        <v>0.1363640136970472</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" s="1" t="n">
-        <v>256</v>
-      </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>[2, 4, 2]</t>
-        </is>
-      </c>
-      <c r="C258" t="n">
-        <v>1.222896771316119</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" s="1" t="n">
-        <v>257</v>
-      </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>[-2, 6, 4]</t>
-        </is>
-      </c>
-      <c r="C259" t="n">
-        <v>0.1504090225488662</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" s="1" t="n">
-        <v>258</v>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>[-1, 6, 6]</t>
-        </is>
-      </c>
-      <c r="C260" t="n">
-        <v>0.1367520722270798</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" s="1" t="n">
-        <v>259</v>
-      </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>[2, 4, 3]</t>
-        </is>
-      </c>
-      <c r="C261" t="n">
-        <v>1.225625200338692</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>[-2, 7, 4]</t>
-        </is>
-      </c>
-      <c r="C262" t="n">
-        <v>0.1313572161811981</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>[1, 4, 0]</t>
-        </is>
-      </c>
-      <c r="C263" t="n">
-        <v>1.28587942960423</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="B264" t="inlineStr">
-        <is>
-          <t>[-1, 7, 6]</t>
-        </is>
-      </c>
-      <c r="C264" t="n">
-        <v>0.1182703776762718</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B265" t="inlineStr">
-        <is>
-          <t>[1, 7, 3]</t>
-        </is>
-      </c>
-      <c r="C265" t="n">
-        <v>0.1275846963339833</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>[1, 7, 2]</t>
-        </is>
-      </c>
-      <c r="C266" t="n">
-        <v>0.1270157024409287</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" s="1" t="n">
-        <v>265</v>
-      </c>
-      <c r="B267" t="inlineStr">
-        <is>
-          <t>[3, 7, 2]</t>
-        </is>
-      </c>
-      <c r="C267" t="n">
-        <v>0.1061116599569736</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" s="1" t="n">
-        <v>266</v>
-      </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>[1, 7, 4]</t>
-        </is>
-      </c>
-      <c r="C268" t="n">
-        <v>0.1251324665740902</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" s="1" t="n">
-        <v>267</v>
-      </c>
-      <c r="B269" t="inlineStr">
-        <is>
-          <t>[0, 6, 4]</t>
-        </is>
-      </c>
-      <c r="C269" t="n">
-        <v>0.1476224777505551</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" s="1" t="n">
-        <v>268</v>
-      </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>[2, 7, 3]</t>
-        </is>
-      </c>
-      <c r="C270" t="n">
-        <v>0.1163878423236481</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" s="1" t="n">
-        <v>269</v>
-      </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>[0, 7, 5]</t>
-        </is>
-      </c>
-      <c r="C271" t="n">
-        <v>0.1238952637500373</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" s="1" t="n">
-        <v>270</v>
-      </c>
-      <c r="B272" t="inlineStr">
-        <is>
-          <t>[-1, 4, 6]</t>
-        </is>
-      </c>
-      <c r="C272" t="n">
-        <v>1.307552990850153</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" s="1" t="n">
-        <v>271</v>
-      </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>[2, 7, 2]</t>
-        </is>
-      </c>
-      <c r="C273" t="n">
-        <v>0.1150221680015083</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" s="1" t="n">
-        <v>272</v>
-      </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>[-1, 5, 6]</t>
-        </is>
-      </c>
-      <c r="C274" t="n">
-        <v>0.4875380746431179</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" s="1" t="n">
-        <v>273</v>
-      </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>[-1, 6, 7]</t>
-        </is>
-      </c>
-      <c r="C275" t="n">
-        <v>0.1301038224100504</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" s="1" t="n">
-        <v>274</v>
-      </c>
-      <c r="B276" t="inlineStr">
-        <is>
-          <t>[0, 6, 6]</t>
-        </is>
-      </c>
-      <c r="C276" t="n">
-        <v>0.1351420412968447</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="B277" t="inlineStr">
-        <is>
-          <t>[-2, 7, 3]</t>
-        </is>
-      </c>
-      <c r="C277" t="n">
-        <v>0.1370100782432043</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" s="1" t="n">
-        <v>276</v>
-      </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>[-2, 6, 5]</t>
-        </is>
-      </c>
-      <c r="C278" t="n">
-        <v>0.143628876642589</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" s="1" t="n">
-        <v>277</v>
-      </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>[1, 6, 4]</t>
-        </is>
-      </c>
-      <c r="C279" t="n">
-        <v>0.1420839058306379</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" s="1" t="n">
-        <v>278</v>
-      </c>
-      <c r="B280" t="inlineStr">
-        <is>
-          <t>[1, 6, 5]</t>
-        </is>
-      </c>
-      <c r="C280" t="n">
-        <v>0.1372421896619689</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" s="1" t="n">
-        <v>279</v>
-      </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>[1, 5, 4]</t>
-        </is>
-      </c>
-      <c r="C281" t="n">
-        <v>0.4853161079156003</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" s="1" t="n">
-        <v>280</v>
-      </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>[-4, 6, 2]</t>
-        </is>
-      </c>
-      <c r="C282" t="n">
-        <v>0.153424885349953</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" s="1" t="n">
-        <v>281</v>
-      </c>
-      <c r="B283" t="inlineStr">
-        <is>
-          <t>[-4, 6, 4]</t>
-        </is>
-      </c>
-      <c r="C283" t="n">
-        <v>0.1441242378458218</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" s="1" t="n">
-        <v>282</v>
-      </c>
-      <c r="B284" t="inlineStr">
-        <is>
-          <t>[0, 5, 4]</t>
-        </is>
-      </c>
-      <c r="C284" t="n">
-        <v>0.4981904668120194</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" s="1" t="n">
-        <v>283</v>
-      </c>
-      <c r="B285" t="inlineStr">
-        <is>
-          <t>[2, 6, 1]</t>
-        </is>
-      </c>
-      <c r="C285" t="n">
-        <v>0.1342063216717148</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" s="1" t="n">
-        <v>284</v>
-      </c>
-      <c r="B286" t="inlineStr">
-        <is>
-          <t>[4, 6, 1]</t>
-        </is>
-      </c>
-      <c r="C286" t="n">
-        <v>0.1181780155362239</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" s="1" t="n">
-        <v>285</v>
-      </c>
-      <c r="B287" t="inlineStr">
-        <is>
-          <t>[4, 6, 2]</t>
-        </is>
-      </c>
-      <c r="C287" t="n">
-        <v>0.1164230145777857</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" s="1" t="n">
-        <v>286</v>
-      </c>
-      <c r="B288" t="inlineStr">
-        <is>
-          <t>[2, 6, 2]</t>
-        </is>
-      </c>
-      <c r="C288" t="n">
-        <v>0.1327901302812185</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" s="1" t="n">
-        <v>287</v>
-      </c>
-      <c r="B289" t="inlineStr">
-        <is>
-          <t>[0, 6, -1]</t>
-        </is>
-      </c>
-      <c r="C289" t="n">
-        <v>0.1446398312319528</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" s="1" t="n">
-        <v>288</v>
-      </c>
-      <c r="B290" t="inlineStr">
-        <is>
-          <t>[0, 6, -2]</t>
-        </is>
-      </c>
-      <c r="C290" t="n">
-        <v>0.1368868779733736</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" s="1" t="n">
-        <v>289</v>
-      </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>[-1, 7, -2]</t>
-        </is>
-      </c>
-      <c r="C291" t="n">
-        <v>0.1231607834801962</v>
+        <v>5.017274400161495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>